<commit_message>
Update INFO files and .gitignore configuration
</commit_message>
<xml_diff>
--- a/INFO/KEY.xlsx
+++ b/INFO/KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6d8442ed8911bd8/Desktop/TraderHelper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="474" documentId="14_{4FB97C0C-97C7-442E-856D-2D1FB01D34EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B53C658-85E1-479B-95BC-4057D19D3DB5}"/>
+  <xr:revisionPtr revIDLastSave="477" documentId="14_{4FB97C0C-97C7-442E-856D-2D1FB01D34EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AD04FE6-7EA1-4F72-A76A-62A7522FBAD7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AE3B0FA6-7D85-412A-8232-C1BDBA7736A9}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="24105" windowHeight="12315" xr2:uid="{AE3B0FA6-7D85-412A-8232-C1BDBA7736A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="89">
   <si>
     <t>ANR-SE-T</t>
   </si>
@@ -350,12 +350,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,10 +369,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -697,7 +691,7 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +728,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="2">
-        <v>0.206875</v>
+        <v>0.23833333333333337</v>
       </c>
       <c r="E2" t="s">
         <v>79</v>
@@ -751,7 +745,7 @@
         <v>45</v>
       </c>
       <c r="D3" s="2">
-        <v>-1.6666666666666676E-3</v>
+        <v>-2.5833333333333333E-2</v>
       </c>
       <c r="E3" t="s">
         <v>78</v>
@@ -768,7 +762,7 @@
         <v>45</v>
       </c>
       <c r="D4" s="2">
-        <v>-0.69499999999999995</v>
+        <v>-0.59</v>
       </c>
       <c r="E4" t="s">
         <v>81</v>
@@ -785,7 +779,7 @@
         <v>35</v>
       </c>
       <c r="D5" s="2">
-        <v>-0.42249999999999999</v>
+        <v>-0.41249999999999998</v>
       </c>
       <c r="E5" t="s">
         <v>77</v>
@@ -819,7 +813,7 @@
         <v>45</v>
       </c>
       <c r="D7" s="2">
-        <v>-0.27166666666666667</v>
+        <v>-0.315</v>
       </c>
       <c r="E7" t="s">
         <v>80</v>
@@ -836,7 +830,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="2">
-        <v>-3.5000000000000003E-2</v>
+        <v>-0.09</v>
       </c>
       <c r="E8" t="s">
         <v>80</v>
@@ -853,7 +847,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="2">
-        <v>-0.40925</v>
+        <v>-0.38116666666666665</v>
       </c>
       <c r="E9" t="s">
         <v>77</v>
@@ -887,7 +881,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="2">
-        <v>-0.81416666666666659</v>
+        <v>-0.94683333333333319</v>
       </c>
       <c r="E11" t="s">
         <v>83</v>
@@ -903,8 +897,8 @@
       <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="4">
-        <v>0.55249999999999988</v>
+      <c r="D12" s="2">
+        <v>0.61083333333333334</v>
       </c>
       <c r="E12" t="s">
         <v>86</v>
@@ -921,7 +915,7 @@
         <v>45</v>
       </c>
       <c r="D13" s="2">
-        <v>2.5000000000000022E-4</v>
+        <v>5.6666666666666671E-3</v>
       </c>
       <c r="E13" t="s">
         <v>80</v>
@@ -938,7 +932,7 @@
         <v>45</v>
       </c>
       <c r="D14" s="2">
-        <v>-0.35499999999999998</v>
+        <v>-0.33500000000000002</v>
       </c>
       <c r="E14" t="s">
         <v>78</v>
@@ -955,7 +949,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="2">
-        <v>-0.35250000000000004</v>
+        <v>-0.29000000000000004</v>
       </c>
       <c r="E15" t="s">
         <v>75</v>
@@ -972,7 +966,7 @@
         <v>34</v>
       </c>
       <c r="D16" s="2">
-        <v>0.43666666666666659</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
         <v>79</v>
@@ -989,7 +983,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="2">
-        <v>-0.81583333333333341</v>
+        <v>-0.93599999999999994</v>
       </c>
       <c r="E17" t="s">
         <v>82</v>
@@ -1006,7 +1000,7 @@
         <v>35</v>
       </c>
       <c r="D18" s="2">
-        <v>-0.40499999999999997</v>
+        <v>-0.39749999999999996</v>
       </c>
       <c r="E18" t="s">
         <v>76</v>
@@ -1040,7 +1034,7 @@
         <v>45</v>
       </c>
       <c r="D20" s="2">
-        <v>-0.53083333333333327</v>
+        <v>-0.55333333333333334</v>
       </c>
       <c r="E20" t="s">
         <v>81</v>
@@ -1057,7 +1051,7 @@
         <v>45</v>
       </c>
       <c r="D21" s="2">
-        <v>-0.34</v>
+        <v>-0.32</v>
       </c>
       <c r="E21" t="s">
         <v>78</v>
@@ -1074,7 +1068,7 @@
         <v>45</v>
       </c>
       <c r="D22" s="2">
-        <v>-0.38500000000000001</v>
+        <v>-0.38083333333333336</v>
       </c>
       <c r="E22" t="s">
         <v>78</v>
@@ -1091,7 +1085,7 @@
         <v>35</v>
       </c>
       <c r="D23" s="2">
-        <v>-0.58583333333333332</v>
+        <v>-0.61166666666666669</v>
       </c>
       <c r="E23" t="s">
         <v>77</v>
@@ -1108,7 +1102,7 @@
         <v>35</v>
       </c>
       <c r="D24" s="2">
-        <v>-0.51666666666666672</v>
+        <v>-0.52249999999999996</v>
       </c>
       <c r="E24" t="s">
         <v>77</v>
@@ -1125,7 +1119,7 @@
         <v>45</v>
       </c>
       <c r="D25" s="2">
-        <v>-0.57750000000000001</v>
+        <v>-0.62</v>
       </c>
       <c r="E25" t="s">
         <v>81</v>
@@ -1142,7 +1136,7 @@
         <v>45</v>
       </c>
       <c r="D26" s="2">
-        <v>-6.0000000000000005E-2</v>
+        <v>-8.1250000000000003E-2</v>
       </c>
       <c r="E26" t="s">
         <v>73</v>
@@ -1159,7 +1153,7 @@
         <v>35</v>
       </c>
       <c r="D27" s="2">
-        <v>0.29749999999999999</v>
+        <v>-0.41000000000000003</v>
       </c>
       <c r="E27" t="s">
         <v>77</v>
@@ -1176,7 +1170,7 @@
         <v>35</v>
       </c>
       <c r="D28" s="2">
-        <v>-0.45999999999999996</v>
+        <v>-0.44425000000000003</v>
       </c>
       <c r="E28" t="s">
         <v>77</v>
@@ -1193,7 +1187,7 @@
         <v>45</v>
       </c>
       <c r="D29" s="2">
-        <v>0.29250000000000004</v>
+        <v>0.37666666666666665</v>
       </c>
       <c r="E29" t="s">
         <v>73</v>
@@ -1210,7 +1204,7 @@
         <v>34</v>
       </c>
       <c r="D30" s="2">
-        <v>-0.61083333333333334</v>
+        <v>-0.64</v>
       </c>
       <c r="E30" t="s">
         <v>83</v>
@@ -1227,7 +1221,7 @@
         <v>45</v>
       </c>
       <c r="D31" s="2">
-        <v>-0.21416666666666664</v>
+        <v>-0.25374999999999998</v>
       </c>
       <c r="E31" t="s">
         <v>78</v>
@@ -1244,7 +1238,7 @@
         <v>34</v>
       </c>
       <c r="D32" s="2">
-        <v>-0.80833333333333324</v>
+        <v>-0.9325</v>
       </c>
       <c r="E32" t="s">
         <v>83</v>
@@ -1261,7 +1255,7 @@
         <v>34</v>
       </c>
       <c r="D33" s="2">
-        <v>-0.6825</v>
+        <v>-0.78766666666666663</v>
       </c>
       <c r="E33" t="s">
         <v>79</v>
@@ -1278,7 +1272,7 @@
         <v>45</v>
       </c>
       <c r="D34" s="2">
-        <v>-0.36</v>
+        <v>-0.34499999999999997</v>
       </c>
       <c r="E34" t="s">
         <v>78</v>
@@ -1295,7 +1289,7 @@
         <v>45</v>
       </c>
       <c r="D35" s="2">
-        <v>-0.1225</v>
+        <v>-9.7499999999999989E-2</v>
       </c>
       <c r="E35" t="s">
         <v>78</v>
@@ -1312,7 +1306,7 @@
         <v>31</v>
       </c>
       <c r="D36" s="2">
-        <v>0.34833333333333333</v>
+        <v>0.448125</v>
       </c>
       <c r="E36" t="s">
         <v>78</v>
@@ -1329,7 +1323,7 @@
         <v>45</v>
       </c>
       <c r="D37" s="2">
-        <v>-0.17666666666666667</v>
+        <v>-0.20083333333333334</v>
       </c>
       <c r="E37" t="s">
         <v>78</v>
@@ -1346,7 +1340,7 @@
         <v>45</v>
       </c>
       <c r="D38" s="2">
-        <v>-0.39250000000000002</v>
+        <v>-0.41850000000000004</v>
       </c>
       <c r="E38" t="s">
         <v>78</v>
@@ -1362,8 +1356,8 @@
       <c r="C39" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>87</v>
+      <c r="D39" s="2">
+        <v>-0.37</v>
       </c>
       <c r="E39" t="s">
         <v>78</v>
@@ -1379,8 +1373,8 @@
       <c r="C40" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>87</v>
+      <c r="D40" s="2">
+        <v>-0.4</v>
       </c>
       <c r="E40" t="s">
         <v>78</v>
@@ -1396,8 +1390,8 @@
       <c r="C41" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>87</v>
+      <c r="D41" s="2">
+        <v>-1.0262500000000001</v>
       </c>
       <c r="E41" t="s">
         <v>83</v>
@@ -1414,7 +1408,7 @@
         <v>34</v>
       </c>
       <c r="D42" s="2">
-        <v>-0.55000000000000004</v>
+        <v>-0.75</v>
       </c>
       <c r="E42" t="s">
         <v>83</v>
@@ -1448,7 +1442,7 @@
         <v>45</v>
       </c>
       <c r="D44" s="2">
-        <v>-0.27</v>
+        <v>-0.3133333333333333</v>
       </c>
       <c r="E44" t="s">
         <v>78</v>
@@ -1464,7 +1458,7 @@
       <c r="C45" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E45" t="s">
@@ -1482,7 +1476,7 @@
         <v>34</v>
       </c>
       <c r="D46" s="2">
-        <v>-0.78</v>
+        <v>-0.94</v>
       </c>
       <c r="E46" t="s">
         <v>85</v>
@@ -1499,7 +1493,7 @@
         <v>45</v>
       </c>
       <c r="D47" s="2">
-        <v>-0.27500000000000002</v>
+        <v>-0.32750000000000001</v>
       </c>
       <c r="E47" t="s">
         <v>78</v>
@@ -1516,7 +1510,7 @@
         <v>45</v>
       </c>
       <c r="D48" s="2">
-        <v>-9.9999999999999992E-2</v>
+        <v>-9.7500000000000003E-2</v>
       </c>
       <c r="E48" t="s">
         <v>73</v>
@@ -1533,7 +1527,7 @@
         <v>45</v>
       </c>
       <c r="D49" s="2">
-        <v>0.17083333333333331</v>
+        <v>0.315</v>
       </c>
       <c r="E49" t="s">
         <v>73</v>
@@ -1550,7 +1544,7 @@
         <v>31</v>
       </c>
       <c r="D50" s="2">
-        <v>0.37</v>
+        <v>0.43125000000000002</v>
       </c>
       <c r="E50" t="s">
         <v>73</v>
@@ -1567,7 +1561,7 @@
         <v>34</v>
       </c>
       <c r="D51" s="2">
-        <v>0.51333333333333331</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="E51" t="s">
         <v>84</v>
@@ -1584,7 +1578,7 @@
         <v>34</v>
       </c>
       <c r="D52" s="2">
-        <v>-0.74374999999999991</v>
+        <v>-0.877</v>
       </c>
       <c r="E52" t="s">
         <v>82</v>
@@ -1601,7 +1595,7 @@
         <v>34</v>
       </c>
       <c r="D53" s="2">
-        <v>-0.74374999999999991</v>
+        <v>-0.877</v>
       </c>
       <c r="E53" t="s">
         <v>82</v>
@@ -1618,7 +1612,7 @@
         <v>34</v>
       </c>
       <c r="D54" s="2">
-        <v>-0.60250000000000004</v>
+        <v>-0.77683333333333326</v>
       </c>
       <c r="E54" t="s">
         <v>79</v>
@@ -1635,7 +1629,7 @@
         <v>34</v>
       </c>
       <c r="D55" s="2">
-        <v>-0.71250000000000002</v>
+        <v>-0.87250000000000005</v>
       </c>
       <c r="E55" t="s">
         <v>82</v>
@@ -1652,7 +1646,7 @@
         <v>45</v>
       </c>
       <c r="D56" s="2">
-        <v>-0.38375000000000004</v>
+        <v>-0.41000000000000003</v>
       </c>
       <c r="E56" t="s">
         <v>78</v>
@@ -1668,8 +1662,8 @@
       <c r="C57" t="s">
         <v>34</v>
       </c>
-      <c r="D57" s="2">
-        <v>-0.4</v>
+      <c r="D57" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="E57" t="s">
         <v>75</v>
@@ -1686,7 +1680,7 @@
         <v>45</v>
       </c>
       <c r="D58" s="2">
-        <v>-2.0425</v>
+        <v>-2.1983333333333333</v>
       </c>
       <c r="E58" t="s">
         <v>78</v>

</xml_diff>